<commit_message>
Minor edits to text
</commit_message>
<xml_diff>
--- a/scheduleFile_template.xlsx
+++ b/scheduleFile_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sjvan\Documents\Soils_Xcutting\DaycentEffort\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sdumb\Dropbox (SSD)\CCRP Daycent Helper\DayCentSchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C7BE128-6902-469C-810E-15670078067C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C13AB05-33DE-41D0-A2BC-352649E874E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{EDBC8291-81B5-48C4-8407-BBAB3CB6D70B}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{EDBC8291-81B5-48C4-8407-BBAB3CB6D70B}"/>
   </bookViews>
   <sheets>
     <sheet name="year 1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="83">
   <si>
     <t>arado de disco</t>
   </si>
@@ -286,6 +286,9 @@
   </si>
   <si>
     <t>CULT HW-7</t>
+  </si>
+  <si>
+    <t>cosecha con exporta de rastrojo 90%</t>
   </si>
 </sst>
 </file>
@@ -701,17 +704,17 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="21.86328125" customWidth="1"/>
+    <col min="3" max="4" width="19.86328125" customWidth="1"/>
+    <col min="5" max="5" width="39.59765625" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="7" max="8" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -731,7 +734,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="7">
         <v>44411</v>
       </c>
@@ -741,7 +744,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A24" si="0">A2+7</f>
         <v>44418</v>
@@ -752,7 +755,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>44425</v>
@@ -763,7 +766,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>44432</v>
@@ -774,7 +777,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>44439</v>
@@ -785,7 +788,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>44446</v>
@@ -796,7 +799,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>44453</v>
@@ -807,7 +810,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>44460</v>
@@ -818,7 +821,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>44467</v>
@@ -829,7 +832,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>44474</v>
@@ -840,7 +843,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>44481</v>
@@ -851,7 +854,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>44488</v>
@@ -862,7 +865,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>44495</v>
@@ -873,7 +876,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>44502</v>
@@ -884,7 +887,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>44509</v>
@@ -895,7 +898,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>44516</v>
@@ -906,7 +909,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>44523</v>
@@ -917,7 +920,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>44530</v>
@@ -928,7 +931,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>44537</v>
@@ -939,7 +942,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>44544</v>
@@ -950,7 +953,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>44551</v>
@@ -961,7 +964,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>44558</v>
@@ -972,7 +975,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>44565</v>
@@ -983,7 +986,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <f t="shared" ref="A25" si="1">A24+7</f>
         <v>44572</v>
@@ -994,7 +997,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <f t="shared" ref="A26:A51" si="2">A25+7</f>
         <v>44579</v>
@@ -1005,7 +1008,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <f t="shared" si="2"/>
         <v>44586</v>
@@ -1016,7 +1019,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <f t="shared" si="2"/>
         <v>44593</v>
@@ -1027,7 +1030,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <f t="shared" si="2"/>
         <v>44600</v>
@@ -1038,7 +1041,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <f t="shared" si="2"/>
         <v>44607</v>
@@ -1049,7 +1052,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <f t="shared" si="2"/>
         <v>44614</v>
@@ -1060,7 +1063,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <f t="shared" si="2"/>
         <v>44621</v>
@@ -1071,7 +1074,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="6">
         <f t="shared" si="2"/>
         <v>44628</v>
@@ -1082,7 +1085,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="6">
         <f t="shared" si="2"/>
         <v>44635</v>
@@ -1093,7 +1096,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="6">
         <f t="shared" si="2"/>
         <v>44642</v>
@@ -1104,7 +1107,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="6">
         <f t="shared" si="2"/>
         <v>44649</v>
@@ -1115,7 +1118,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="6">
         <f t="shared" si="2"/>
         <v>44656</v>
@@ -1126,7 +1129,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="6">
         <f t="shared" si="2"/>
         <v>44663</v>
@@ -1137,7 +1140,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="6">
         <f t="shared" si="2"/>
         <v>44670</v>
@@ -1148,7 +1151,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="6">
         <f t="shared" si="2"/>
         <v>44677</v>
@@ -1159,7 +1162,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="6">
         <f t="shared" si="2"/>
         <v>44684</v>
@@ -1170,7 +1173,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="6">
         <f t="shared" si="2"/>
         <v>44691</v>
@@ -1181,7 +1184,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="6">
         <f t="shared" si="2"/>
         <v>44698</v>
@@ -1192,7 +1195,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="6">
         <f t="shared" si="2"/>
         <v>44705</v>
@@ -1203,7 +1206,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="6">
         <f t="shared" si="2"/>
         <v>44712</v>
@@ -1214,7 +1217,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="6">
         <f t="shared" si="2"/>
         <v>44719</v>
@@ -1225,7 +1228,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="6">
         <f t="shared" si="2"/>
         <v>44726</v>
@@ -1236,7 +1239,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="6">
         <f t="shared" si="2"/>
         <v>44733</v>
@@ -1247,7 +1250,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="6">
         <f t="shared" si="2"/>
         <v>44740</v>
@@ -1258,7 +1261,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="6">
         <f t="shared" si="2"/>
         <v>44747</v>
@@ -1269,7 +1272,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="6">
         <f t="shared" si="2"/>
         <v>44754</v>
@@ -1280,7 +1283,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="6">
         <f t="shared" ref="A52" si="3">A51+7</f>
         <v>44761</v>
@@ -1291,7 +1294,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="6">
         <f>A52+7</f>
         <v>44768</v>
@@ -1302,55 +1305,55 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="4"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="4"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="4"/>
     </row>
   </sheetData>
@@ -1402,22 +1405,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B73A2E7-7F61-4FC6-ACF5-DEC31DEDF09F}">
   <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" customWidth="1"/>
-    <col min="4" max="4" width="30.85546875" customWidth="1"/>
-    <col min="5" max="5" width="44.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.85546875" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.86328125" style="5" customWidth="1"/>
+    <col min="2" max="2" width="27.265625" customWidth="1"/>
+    <col min="3" max="3" width="28.1328125" customWidth="1"/>
+    <col min="4" max="4" width="30.86328125" customWidth="1"/>
+    <col min="5" max="5" width="44.265625" customWidth="1"/>
+    <col min="6" max="6" width="28.86328125" customWidth="1"/>
+    <col min="7" max="8" width="9.1328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.5">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1437,7 +1440,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="7">
         <v>44776</v>
       </c>
@@ -1447,7 +1450,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="6">
         <f t="shared" ref="A3:A52" si="0">A2+7</f>
         <v>44783</v>
@@ -1458,7 +1461,7 @@
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
         <f t="shared" si="0"/>
         <v>44790</v>
@@ -1469,7 +1472,7 @@
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
         <f t="shared" si="0"/>
         <v>44797</v>
@@ -1480,7 +1483,7 @@
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
         <f t="shared" si="0"/>
         <v>44804</v>
@@ -1491,7 +1494,7 @@
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
         <f t="shared" si="0"/>
         <v>44811</v>
@@ -1502,7 +1505,7 @@
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="6">
         <f t="shared" si="0"/>
         <v>44818</v>
@@ -1513,7 +1516,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="6">
         <f t="shared" si="0"/>
         <v>44825</v>
@@ -1524,7 +1527,7 @@
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="6">
         <f t="shared" si="0"/>
         <v>44832</v>
@@ -1535,7 +1538,7 @@
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="6">
         <f t="shared" si="0"/>
         <v>44839</v>
@@ -1546,7 +1549,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="6">
         <f t="shared" si="0"/>
         <v>44846</v>
@@ -1557,7 +1560,7 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="6">
         <f t="shared" si="0"/>
         <v>44853</v>
@@ -1568,7 +1571,7 @@
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6">
         <f t="shared" si="0"/>
         <v>44860</v>
@@ -1579,7 +1582,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="6">
         <f t="shared" si="0"/>
         <v>44867</v>
@@ -1590,7 +1593,7 @@
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="6">
         <f t="shared" si="0"/>
         <v>44874</v>
@@ -1601,7 +1604,7 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="6">
         <f t="shared" si="0"/>
         <v>44881</v>
@@ -1612,7 +1615,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="6">
         <f t="shared" si="0"/>
         <v>44888</v>
@@ -1623,7 +1626,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="6">
         <f t="shared" si="0"/>
         <v>44895</v>
@@ -1634,7 +1637,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="6">
         <f t="shared" si="0"/>
         <v>44902</v>
@@ -1645,7 +1648,7 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="6">
         <f t="shared" si="0"/>
         <v>44909</v>
@@ -1656,7 +1659,7 @@
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="6">
         <f t="shared" si="0"/>
         <v>44916</v>
@@ -1667,7 +1670,7 @@
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="6">
         <f t="shared" si="0"/>
         <v>44923</v>
@@ -1678,7 +1681,7 @@
       <c r="E23" s="8"/>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="6">
         <f t="shared" si="0"/>
         <v>44930</v>
@@ -1689,7 +1692,7 @@
       <c r="E24" s="8"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="6">
         <f t="shared" si="0"/>
         <v>44937</v>
@@ -1700,7 +1703,7 @@
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="6">
         <f t="shared" si="0"/>
         <v>44944</v>
@@ -1711,7 +1714,7 @@
       <c r="E26" s="8"/>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="6">
         <f t="shared" si="0"/>
         <v>44951</v>
@@ -1722,7 +1725,7 @@
       <c r="E27" s="8"/>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="6">
         <f t="shared" si="0"/>
         <v>44958</v>
@@ -1733,7 +1736,7 @@
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="6">
         <f t="shared" si="0"/>
         <v>44965</v>
@@ -1744,7 +1747,7 @@
       <c r="E29" s="8"/>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="6">
         <f t="shared" si="0"/>
         <v>44972</v>
@@ -1755,7 +1758,7 @@
       <c r="E30" s="8"/>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="6">
         <f t="shared" si="0"/>
         <v>44979</v>
@@ -1766,7 +1769,7 @@
       <c r="E31" s="8"/>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="6">
         <f t="shared" si="0"/>
         <v>44986</v>
@@ -1777,7 +1780,7 @@
       <c r="E32" s="8"/>
       <c r="F32" s="8"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="6">
         <f t="shared" si="0"/>
         <v>44993</v>
@@ -1788,7 +1791,7 @@
       <c r="E33" s="8"/>
       <c r="F33" s="8"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="6">
         <f t="shared" si="0"/>
         <v>45000</v>
@@ -1799,7 +1802,7 @@
       <c r="E34" s="8"/>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="6">
         <f t="shared" si="0"/>
         <v>45007</v>
@@ -1810,7 +1813,7 @@
       <c r="E35" s="8"/>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="6">
         <f t="shared" si="0"/>
         <v>45014</v>
@@ -1821,7 +1824,7 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="6">
         <f t="shared" si="0"/>
         <v>45021</v>
@@ -1832,7 +1835,7 @@
       <c r="E37" s="8"/>
       <c r="F37" s="8"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="6">
         <f t="shared" si="0"/>
         <v>45028</v>
@@ -1843,7 +1846,7 @@
       <c r="E38" s="8"/>
       <c r="F38" s="8"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="6">
         <f t="shared" si="0"/>
         <v>45035</v>
@@ -1854,7 +1857,7 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="6">
         <f t="shared" si="0"/>
         <v>45042</v>
@@ -1865,7 +1868,7 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="6">
         <f t="shared" si="0"/>
         <v>45049</v>
@@ -1876,7 +1879,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="6">
         <f t="shared" si="0"/>
         <v>45056</v>
@@ -1887,7 +1890,7 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="6">
         <f t="shared" si="0"/>
         <v>45063</v>
@@ -1898,7 +1901,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="6">
         <f t="shared" si="0"/>
         <v>45070</v>
@@ -1909,7 +1912,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="6">
         <f t="shared" si="0"/>
         <v>45077</v>
@@ -1920,7 +1923,7 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="6">
         <f t="shared" si="0"/>
         <v>45084</v>
@@ -1931,7 +1934,7 @@
       <c r="E46" s="8"/>
       <c r="F46" s="8"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="6">
         <f t="shared" si="0"/>
         <v>45091</v>
@@ -1942,7 +1945,7 @@
       <c r="E47" s="8"/>
       <c r="F47" s="8"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="6">
         <f t="shared" si="0"/>
         <v>45098</v>
@@ -1953,7 +1956,7 @@
       <c r="E48" s="8"/>
       <c r="F48" s="8"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="6">
         <f t="shared" si="0"/>
         <v>45105</v>
@@ -1964,7 +1967,7 @@
       <c r="E49" s="8"/>
       <c r="F49" s="8"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="6">
         <f t="shared" si="0"/>
         <v>45112</v>
@@ -1975,7 +1978,7 @@
       <c r="E50" s="8"/>
       <c r="F50" s="8"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="6">
         <f t="shared" si="0"/>
         <v>45119</v>
@@ -1986,7 +1989,7 @@
       <c r="E51" s="8"/>
       <c r="F51" s="8"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="6">
         <f t="shared" si="0"/>
         <v>45126</v>
@@ -1997,7 +2000,7 @@
       <c r="E52" s="8"/>
       <c r="F52" s="8"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="6">
         <f>A52+7</f>
         <v>45133</v>
@@ -2008,55 +2011,55 @@
       <c r="E53" s="8"/>
       <c r="F53" s="8"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="4"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="4"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="4"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="4"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="4"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="4"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="4"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="4"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="4"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="4"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="4"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A65" s="4"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A66" s="4"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A67" s="4"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A68" s="4"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A69" s="4"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A70" s="4"/>
     </row>
   </sheetData>
@@ -2107,19 +2110,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA84CE52-E379-435C-8752-A005ED882610}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="42.59765625" customWidth="1"/>
+    <col min="2" max="2" width="29.1328125" customWidth="1"/>
+    <col min="3" max="3" width="11.265625" customWidth="1"/>
+    <col min="4" max="4" width="13.86328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>13</v>
       </c>
@@ -2130,12 +2133,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="9"/>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
         <v>33</v>
       </c>
@@ -2146,7 +2149,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
         <v>22</v>
       </c>
@@ -2157,7 +2160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="9" t="s">
         <v>75</v>
       </c>
@@ -2179,7 +2182,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="9" t="s">
         <v>76</v>
       </c>
@@ -2190,7 +2193,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="9" t="s">
         <v>1</v>
       </c>
@@ -2201,12 +2204,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2217,7 +2220,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="9" t="s">
         <v>23</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>24</v>
       </c>
@@ -2239,12 +2242,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="9" t="s">
         <v>6</v>
       </c>
@@ -2255,7 +2258,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="9" t="s">
         <v>7</v>
       </c>
@@ -2266,7 +2269,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="9" t="s">
         <v>8</v>
       </c>
@@ -2277,7 +2280,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="9" t="s">
         <v>9</v>
       </c>
@@ -2288,7 +2291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -2299,7 +2302,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="9" t="s">
         <v>34</v>
       </c>
@@ -2310,7 +2313,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>11</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="9" t="s">
         <v>12</v>
       </c>
@@ -2332,7 +2335,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>77</v>
       </c>
@@ -2343,7 +2346,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="9" t="s">
         <v>78</v>
       </c>
@@ -2354,12 +2357,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="9" t="s">
         <v>43</v>
       </c>
@@ -2370,7 +2373,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="9" t="s">
         <v>35</v>
       </c>
@@ -2381,7 +2384,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="9" t="s">
         <v>37</v>
       </c>
@@ -2392,9 +2395,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="9" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>40</v>
@@ -2403,7 +2406,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="9" t="s">
         <v>41</v>
       </c>
@@ -2414,7 +2417,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="9" t="s">
         <v>3</v>
       </c>
@@ -2425,12 +2428,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A32" s="9" t="s">
         <v>47</v>
       </c>
@@ -2441,7 +2444,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" s="9" t="s">
         <v>48</v>
       </c>
@@ -2452,7 +2455,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" s="9" t="s">
         <v>44</v>
       </c>
@@ -2463,7 +2466,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" s="9" t="s">
         <v>46</v>
       </c>
@@ -2474,7 +2477,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" s="9" t="s">
         <v>45</v>
       </c>
@@ -2485,7 +2488,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" s="9" t="s">
         <v>53</v>
       </c>
@@ -2496,7 +2499,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" s="9" t="s">
         <v>54</v>
       </c>
@@ -2507,7 +2510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" s="9" t="s">
         <v>55</v>
       </c>
@@ -2518,7 +2521,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" s="9" t="s">
         <v>56</v>
       </c>
@@ -2529,7 +2532,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" s="9" t="s">
         <v>57</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" s="9" t="s">
         <v>58</v>
       </c>
@@ -2551,7 +2554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" s="9" t="s">
         <v>59</v>
       </c>

</xml_diff>